<commit_message>
Yr12/Cert III attainment widget.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_yr12_2015_uploader/education_yr12_2015.xlsx
+++ b/dashboard_loader/education_yr12_2015_uploader/education_yr12_2015.xlsx
@@ -141,36 +141,7 @@
     <t xml:space="preserve">Short title</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Lift the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Year 12 or equivalent or</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Certificate II attainment rate</t>
-    </r>
+    <t xml:space="preserve">Lift the Year 12 or equivalent or Certificate II attainment rate</t>
   </si>
   <si>
     <t xml:space="preserve">Status</t>
@@ -216,7 +187,7 @@
     <numFmt numFmtId="172" formatCode="0.000000_ ;\-0.000000\ "/>
     <numFmt numFmtId="173" formatCode="0.000_ ;\-0.000\ "/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -300,13 +271,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -673,7 +637,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3469,7 +3433,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3487,7 +3451,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
         <v>32</v>
       </c>

</xml_diff>